<commit_message>
Historic Storm Surge Aggregation
Historic Storm Surge Aggregation for texas from 2001-2022, 23 storms of cat>0
</commit_message>
<xml_diff>
--- a/Sajjad_Test/Results/all_storm_info.xlsx
+++ b/Sajjad_Test/Results/all_storm_info.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sajjad_Work\Projects\Project_Climada_Hazard\Sajjad_Test\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sajjad_Work\Projects\Project_Climada_Hazard\Hurricane_Flood_WSU\Branch-Sajjad\Hurricane_Flood_WSU\Sajjad_Test\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22CA0AB-EA9D-42CC-9C85-E7D61016553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69F421-F05D-422B-83A3-8EED85AD84C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C004A0A4-F1E4-4914-8050-3B9ED32D824C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Texas" sheetId="2" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">All!$A$1:$E$328</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="536">
   <si>
     <t>Storm ID</t>
   </si>
@@ -1502,58 +1506,148 @@
     <t>MINDY</t>
   </si>
   <si>
+    <t>NICHOLAS</t>
+  </si>
+  <si>
+    <t>2022154N21273</t>
+  </si>
+  <si>
+    <t>2022232N20266</t>
+  </si>
+  <si>
+    <t>2022266N12294</t>
+  </si>
+  <si>
+    <t>IAN</t>
+  </si>
+  <si>
+    <t>2022285N19266</t>
+  </si>
+  <si>
+    <t>2022304N16287</t>
+  </si>
+  <si>
+    <t>LISA</t>
+  </si>
+  <si>
+    <t>2022311N21293</t>
+  </si>
+  <si>
+    <t>NICOLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Longitude </t>
+  </si>
+  <si>
+    <t>Right Longitude</t>
+  </si>
+  <si>
+    <t>Sabine Lake</t>
+  </si>
+  <si>
+    <t>Galveston Bay</t>
+  </si>
+  <si>
+    <t>Matagorda Bay</t>
+  </si>
+  <si>
+    <t>Corpus Christi Bay</t>
+  </si>
+  <si>
+    <t>Laguna Madre</t>
+  </si>
+  <si>
     <t>2021256N21265</t>
   </si>
   <si>
-    <t>NICHOLAS</t>
-  </si>
-  <si>
-    <t>2022154N21273</t>
-  </si>
-  <si>
-    <t>2022232N20266</t>
-  </si>
-  <si>
-    <t>2022266N12294</t>
-  </si>
-  <si>
-    <t>IAN</t>
-  </si>
-  <si>
-    <t>2022285N19266</t>
-  </si>
-  <si>
-    <t>2022304N16287</t>
-  </si>
-  <si>
-    <t>LISA</t>
-  </si>
-  <si>
-    <t>2022311N21293</t>
-  </si>
-  <si>
-    <t>NICOLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left Longitude </t>
-  </si>
-  <si>
-    <t>Right Longitude</t>
-  </si>
-  <si>
-    <t>Sabine Lake</t>
-  </si>
-  <si>
-    <t>Galveston Bay</t>
-  </si>
-  <si>
-    <t>Matagorda Bay</t>
-  </si>
-  <si>
-    <t>Corpus Christi Bay</t>
-  </si>
-  <si>
-    <t>Laguna Madre</t>
+    <t>storm id</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>category at landfall</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>basin</t>
+  </si>
+  <si>
+    <t>n','nnw', 'nw'</t>
+  </si>
+  <si>
+    <t>n','nne'</t>
+  </si>
+  <si>
+    <t>nne','ne'</t>
+  </si>
+  <si>
+    <t>w','wsw'</t>
+  </si>
+  <si>
+    <t>nnw','nw'</t>
+  </si>
+  <si>
+    <t>wsw'</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>nw',nnw'</t>
+  </si>
+  <si>
+    <t>ne','ene'</t>
+  </si>
+  <si>
+    <t>ene'</t>
+  </si>
+  <si>
+    <t>nnw'</t>
+  </si>
+  <si>
+    <t>ne'</t>
+  </si>
+  <si>
+    <t>w','wnw'</t>
+  </si>
+  <si>
+    <t>Ike</t>
+  </si>
+  <si>
+    <t>nw','nnw'</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>nw','wnw'</t>
+  </si>
+  <si>
+    <t>w'</t>
+  </si>
+  <si>
+    <t>Rita</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Katrina</t>
+  </si>
+  <si>
+    <t>w', wnw'</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n', 'nen', </t>
+  </si>
+  <si>
+    <t>Ivan</t>
   </si>
 </sst>
 </file>
@@ -1569,12 +1663,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1589,8 +1689,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1904,11 +2006,390 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02C8BBB-B356-418B-99E4-990AA12B151E}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>530</v>
+      </c>
+      <c r="E5" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E6" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="E12" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E18" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8CE09E-B6FC-474D-AAC8-60166D6A8D77}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="C219" activeCellId="25" sqref="A219 A233 A237:A238 A245:A253 A258 A263 A270 A276:A288 A292:A293 A295 A300:A308 A313 A322 C322 C313 C300:C308 C295 C292:C293 C276:C288 C270 C263 C258 C245:C253 C237:C238 C233 C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,10 +2412,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>498</v>
+      </c>
+      <c r="E1" t="s">
         <v>499</v>
-      </c>
-      <c r="E1" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -1954,7 +2435,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1994,7 +2475,7 @@
         <v>91.8</v>
       </c>
       <c r="W4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -2020,7 +2501,7 @@
         <v>92.9</v>
       </c>
       <c r="W5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -2046,7 +2527,7 @@
         <v>93.4</v>
       </c>
       <c r="W6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -2072,7 +2553,7 @@
         <v>96</v>
       </c>
       <c r="W7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2098,7 +2579,7 @@
         <v>95.6</v>
       </c>
       <c r="W8" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -2322,7 +2803,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2373,7 +2854,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2390,7 +2871,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2407,7 +2888,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2424,7 +2905,7 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2458,7 +2939,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -2509,7 +2990,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -2560,7 +3041,7 @@
         <v>93.5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2662,7 +3143,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2883,7 +3364,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -2934,7 +3415,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -2951,7 +3432,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -3019,7 +3500,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -3053,7 +3534,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -3087,7 +3568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -3138,7 +3619,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>89</v>
       </c>
@@ -3155,7 +3636,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -3189,7 +3670,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>95</v>
       </c>
@@ -3206,7 +3687,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>97</v>
       </c>
@@ -3223,7 +3704,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>99</v>
       </c>
@@ -3274,7 +3755,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>104</v>
       </c>
@@ -3308,7 +3789,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>108</v>
       </c>
@@ -3342,7 +3823,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>111</v>
       </c>
@@ -3393,7 +3874,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>117</v>
       </c>
@@ -3427,7 +3908,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>120</v>
       </c>
@@ -3444,7 +3925,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>122</v>
       </c>
@@ -3461,7 +3942,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>124</v>
       </c>
@@ -3478,7 +3959,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>125</v>
       </c>
@@ -3529,7 +4010,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>129</v>
       </c>
@@ -3563,7 +4044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>132</v>
       </c>
@@ -3580,7 +4061,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>134</v>
       </c>
@@ -3614,7 +4095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>137</v>
       </c>
@@ -3631,7 +4112,7 @@
         <v>81.5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>138</v>
       </c>
@@ -3709,7 +4190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>147</v>
       </c>
@@ -3742,7 +4223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>152</v>
       </c>
@@ -3753,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>153</v>
       </c>
@@ -3786,7 +4267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>158</v>
       </c>
@@ -3819,7 +4300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>163</v>
       </c>
@@ -3830,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>165</v>
       </c>
@@ -3863,7 +4344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>170</v>
       </c>
@@ -3907,7 +4388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>177</v>
       </c>
@@ -3918,7 +4399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>179</v>
       </c>
@@ -3962,7 +4443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>186</v>
       </c>
@@ -3973,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>187</v>
       </c>
@@ -4006,7 +4487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>193</v>
       </c>
@@ -4017,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>195</v>
       </c>
@@ -4028,7 +4509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>197</v>
       </c>
@@ -4050,7 +4531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>200</v>
       </c>
@@ -4072,7 +4553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>204</v>
       </c>
@@ -4105,7 +4586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>210</v>
       </c>
@@ -4116,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>212</v>
       </c>
@@ -4160,7 +4641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>220</v>
       </c>
@@ -4171,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>221</v>
       </c>
@@ -4204,7 +4685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>227</v>
       </c>
@@ -4292,7 +4773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>241</v>
       </c>
@@ -4314,7 +4795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>244</v>
       </c>
@@ -4369,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>253</v>
       </c>
@@ -4413,7 +4894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>261</v>
       </c>
@@ -4424,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>263</v>
       </c>
@@ -4435,7 +4916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>265</v>
       </c>
@@ -4457,7 +4938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>268</v>
       </c>
@@ -4479,7 +4960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>271</v>
       </c>
@@ -4490,7 +4971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>272</v>
       </c>
@@ -4501,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>273</v>
       </c>
@@ -4512,7 +4993,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>274</v>
       </c>
@@ -4545,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>278</v>
       </c>
@@ -4567,7 +5048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>282</v>
       </c>
@@ -4578,7 +5059,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>283</v>
       </c>
@@ -4589,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>285</v>
       </c>
@@ -4633,7 +5114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>292</v>
       </c>
@@ -4655,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>295</v>
       </c>
@@ -4677,7 +5158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>298</v>
       </c>
@@ -4699,7 +5180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>302</v>
       </c>
@@ -4721,7 +5202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>305</v>
       </c>
@@ -4743,7 +5224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>308</v>
       </c>
@@ -4754,7 +5235,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>309</v>
       </c>
@@ -4765,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>311</v>
       </c>
@@ -4787,7 +5268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>313</v>
       </c>
@@ -4798,7 +5279,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>314</v>
       </c>
@@ -4809,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>315</v>
       </c>
@@ -4831,7 +5312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>317</v>
       </c>
@@ -4853,7 +5334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>320</v>
       </c>
@@ -4864,7 +5345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>321</v>
       </c>
@@ -4886,7 +5367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>323</v>
       </c>
@@ -4897,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>324</v>
       </c>
@@ -4908,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>325</v>
       </c>
@@ -4919,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>327</v>
       </c>
@@ -4952,7 +5433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>333</v>
       </c>
@@ -4964,7 +5445,7 @@
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="A219" s="1" t="s">
         <v>335</v>
       </c>
       <c r="B219" t="s">
@@ -4985,7 +5466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>338</v>
       </c>
@@ -4996,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>340</v>
       </c>
@@ -5007,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>341</v>
       </c>
@@ -5018,7 +5499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>343</v>
       </c>
@@ -5062,7 +5543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>348</v>
       </c>
@@ -5073,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>350</v>
       </c>
@@ -5084,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>351</v>
       </c>
@@ -5118,7 +5599,7 @@
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+      <c r="A233" s="1" t="s">
         <v>354</v>
       </c>
       <c r="B233" t="s">
@@ -5128,7 +5609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>356</v>
       </c>
@@ -5139,7 +5620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>357</v>
       </c>
@@ -5162,7 +5643,7 @@
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+      <c r="A237" s="1" t="s">
         <v>361</v>
       </c>
       <c r="B237" t="s">
@@ -5173,7 +5654,7 @@
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
+      <c r="A238" s="1" t="s">
         <v>363</v>
       </c>
       <c r="B238" t="s">
@@ -5194,7 +5675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>367</v>
       </c>
@@ -5216,7 +5697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>370</v>
       </c>
@@ -5238,7 +5719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>372</v>
       </c>
@@ -5250,7 +5731,7 @@
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
+      <c r="A245" s="1" t="s">
         <v>373</v>
       </c>
       <c r="B245" t="s">
@@ -5260,7 +5741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>375</v>
       </c>
@@ -5272,7 +5753,7 @@
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
+      <c r="A247" s="1" t="s">
         <v>376</v>
       </c>
       <c r="B247" t="s">
@@ -5282,7 +5763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>378</v>
       </c>
@@ -5294,7 +5775,7 @@
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
+      <c r="A249" s="1" t="s">
         <v>380</v>
       </c>
       <c r="B249" t="s">
@@ -5304,7 +5785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>381</v>
       </c>
@@ -5315,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>382</v>
       </c>
@@ -5327,7 +5808,7 @@
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
+      <c r="A252" s="1" t="s">
         <v>383</v>
       </c>
       <c r="B252" t="s">
@@ -5338,7 +5819,7 @@
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
+      <c r="A253" s="1" t="s">
         <v>385</v>
       </c>
       <c r="B253" t="s">
@@ -5348,7 +5829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>387</v>
       </c>
@@ -5370,7 +5851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>390</v>
       </c>
@@ -5393,7 +5874,7 @@
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
+      <c r="A258" s="1" t="s">
         <v>393</v>
       </c>
       <c r="B258" t="s">
@@ -5403,7 +5884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>395</v>
       </c>
@@ -5414,7 +5895,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>396</v>
       </c>
@@ -5425,7 +5906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>397</v>
       </c>
@@ -5436,7 +5917,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>398</v>
       </c>
@@ -5448,7 +5929,7 @@
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
+      <c r="A263" s="1" t="s">
         <v>399</v>
       </c>
       <c r="B263" t="s">
@@ -5480,7 +5961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>405</v>
       </c>
@@ -5491,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>406</v>
       </c>
@@ -5502,7 +5983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>408</v>
       </c>
@@ -5513,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>409</v>
       </c>
@@ -5525,7 +6006,7 @@
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
+      <c r="A270" s="1" t="s">
         <v>411</v>
       </c>
       <c r="B270" t="s">
@@ -5546,7 +6027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>415</v>
       </c>
@@ -5568,7 +6049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>417</v>
       </c>
@@ -5591,7 +6072,7 @@
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
+      <c r="A276" s="1" t="s">
         <v>420</v>
       </c>
       <c r="B276" t="s">
@@ -5601,7 +6082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>421</v>
       </c>
@@ -5612,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>423</v>
       </c>
@@ -5623,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>424</v>
       </c>
@@ -5634,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>426</v>
       </c>
@@ -5646,7 +6127,7 @@
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
+      <c r="A281" s="1" t="s">
         <v>427</v>
       </c>
       <c r="B281" t="s">
@@ -5656,7 +6137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>429</v>
       </c>
@@ -5667,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>431</v>
       </c>
@@ -5678,7 +6159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>432</v>
       </c>
@@ -5689,7 +6170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>433</v>
       </c>
@@ -5700,7 +6181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>434</v>
       </c>
@@ -5711,7 +6192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>436</v>
       </c>
@@ -5723,7 +6204,7 @@
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+      <c r="A288" s="1" t="s">
         <v>437</v>
       </c>
       <c r="B288" t="s">
@@ -5744,7 +6225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>439</v>
       </c>
@@ -5755,7 +6236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>440</v>
       </c>
@@ -5767,7 +6248,7 @@
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
+      <c r="A292" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B292" t="s">
@@ -5778,7 +6259,7 @@
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
+      <c r="A293" s="1" t="s">
         <v>443</v>
       </c>
       <c r="B293" t="s">
@@ -5800,7 +6281,7 @@
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
+      <c r="A295" s="1" t="s">
         <v>446</v>
       </c>
       <c r="B295" t="s">
@@ -5821,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>449</v>
       </c>
@@ -5832,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>450</v>
       </c>
@@ -5855,7 +6336,7 @@
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
+      <c r="A300" s="1" t="s">
         <v>453</v>
       </c>
       <c r="B300" t="s">
@@ -5865,7 +6346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>454</v>
       </c>
@@ -5876,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>455</v>
       </c>
@@ -5887,7 +6368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>457</v>
       </c>
@@ -5898,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>459</v>
       </c>
@@ -5909,7 +6390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>460</v>
       </c>
@@ -5920,7 +6401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>462</v>
       </c>
@@ -5932,7 +6413,7 @@
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
+      <c r="A307" s="1" t="s">
         <v>463</v>
       </c>
       <c r="B307" t="s">
@@ -5943,7 +6424,7 @@
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
+      <c r="A308" s="1" t="s">
         <v>464</v>
       </c>
       <c r="B308" t="s">
@@ -5975,7 +6456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>469</v>
       </c>
@@ -5998,7 +6479,7 @@
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
+      <c r="A313" s="1" t="s">
         <v>473</v>
       </c>
       <c r="B313" t="s">
@@ -6030,7 +6511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>479</v>
       </c>
@@ -6052,7 +6533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>482</v>
       </c>
@@ -6085,7 +6566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>486</v>
       </c>
@@ -6097,19 +6578,19 @@
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
+      <c r="A322" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B322" t="s">
         <v>488</v>
       </c>
-      <c r="B322" t="s">
+      <c r="C322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
         <v>489</v>
-      </c>
-      <c r="C322">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
-        <v>490</v>
       </c>
       <c r="B323" t="s">
         <v>394</v>
@@ -6118,9 +6599,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B324" t="s">
         <v>4</v>
@@ -6131,18 +6612,18 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
+        <v>491</v>
+      </c>
+      <c r="B325" t="s">
         <v>492</v>
-      </c>
-      <c r="B325" t="s">
-        <v>493</v>
       </c>
       <c r="C325">
         <v>5</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B326" t="s">
         <v>400</v>
@@ -6153,10 +6634,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
+        <v>494</v>
+      </c>
+      <c r="B327" t="s">
         <v>495</v>
-      </c>
-      <c r="B327" t="s">
-        <v>496</v>
       </c>
       <c r="C327">
         <v>1</v>
@@ -6164,16 +6645,27 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
+        <v>496</v>
+      </c>
+      <c r="B328" t="s">
         <v>497</v>
       </c>
-      <c r="B328" t="s">
-        <v>498</v>
-      </c>
       <c r="C328">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E328" xr:uid="{0C8CE09E-B6FC-474D-AAC8-60166D6A8D77}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="3"/>
+        <filter val="4"/>
+        <filter val="5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing bug in average depth computation
Previously, in case of the presence of garbage values (99.9) in  a row, it was considered while taking the average/maximum which is wrong.

This is fixed, now the output type is like below:
for N=5
the average depth of 99.9, 99.9, 99.9, 99.9, 99.9 is 99.9
the average depth of 99.9, 2, 4, 6, 99.9  is (2+4+6)/5 = 2.4
the average depth of 1, 2, 3, 4, 5 is  (1+2+3+4+5)/5 = 3

All the PESGM 2024 files have been recreated
</commit_message>
<xml_diff>
--- a/Sajjad_Test/Results/all_storm_info.xlsx
+++ b/Sajjad_Test/Results/all_storm_info.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sajjad_Work\Projects\Project_Climada_Hazard\Hurricane_Flood_WSU\Branch-Sajjad\Hurricane_Flood_WSU\Sajjad_Test\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69F421-F05D-422B-83A3-8EED85AD84C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E783FE-6D40-4990-899A-DBA5F2702F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C004A0A4-F1E4-4914-8050-3B9ED32D824C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C004A0A4-F1E4-4914-8050-3B9ED32D824C}"/>
   </bookViews>
   <sheets>
     <sheet name="Texas" sheetId="2" r:id="rId1"/>
     <sheet name="All" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">All!$A$1:$E$328</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="560">
   <si>
     <t>Storm ID</t>
   </si>
@@ -1648,13 +1650,85 @@
   </si>
   <si>
     <t>Ivan</t>
+  </si>
+  <si>
+    <t>NOT NAMED</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>nw,wnw,nnw,n,w</t>
+  </si>
+  <si>
+    <t>n,nnw</t>
+  </si>
+  <si>
+    <t>w,wnw,nw,nnw,n</t>
+  </si>
+  <si>
+    <t>nw,wnw,nnw</t>
+  </si>
+  <si>
+    <t>wnw,nw,nnw</t>
+  </si>
+  <si>
+    <t>n,nne</t>
+  </si>
+  <si>
+    <t>n,nnw,nw</t>
+  </si>
+  <si>
+    <t>nw,nnw,wnw</t>
+  </si>
+  <si>
+    <t>w,wnw</t>
+  </si>
+  <si>
+    <t>e,ene,ne,nne,n</t>
+  </si>
+  <si>
+    <t>nw,nnw,n,wnw</t>
+  </si>
+  <si>
+    <t>w,wnw,nw</t>
+  </si>
+  <si>
+    <t>w,wsw</t>
+  </si>
+  <si>
+    <t>w, wnw</t>
+  </si>
+  <si>
+    <t>nnw,nw</t>
+  </si>
+  <si>
+    <t>nw,nnw</t>
+  </si>
+  <si>
+    <t>Gustav</t>
+  </si>
+  <si>
+    <t>Humberto</t>
+  </si>
+  <si>
+    <t>nne,ne</t>
+  </si>
+  <si>
+    <t>nw,wnw</t>
+  </si>
+  <si>
+    <t>Dolly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1662,8 +1736,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1676,8 +1771,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1685,20 +1792,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF800000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2009,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02C8BBB-B356-418B-99E4-990AA12B151E}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,6 +2302,9 @@
       <c r="D8" s="2" t="s">
         <v>513</v>
       </c>
+      <c r="E8" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2174,6 +2333,9 @@
       <c r="D10" s="2" t="s">
         <v>527</v>
       </c>
+      <c r="E10" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2187,6 +2349,9 @@
       </c>
       <c r="D11" t="s">
         <v>526</v>
+      </c>
+      <c r="E11" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2388,13 +2553,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W328"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="C219" activeCellId="25" sqref="A219 A233 A237:A238 A245:A253 A258 A263 A270 A276:A288 A292:A293 A295 A300:A308 A313 A322 C322 C313 C300:C308 C295 C292:C293 C276:C288 C270 C263 C258 C245:C253 C237:C238 C233 C219"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
@@ -6668,4 +6833,560 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABE162C-3E71-4B29-BE00-14CBD10FB053}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B3" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>540</v>
+      </c>
+      <c r="D3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>541</v>
+      </c>
+      <c r="D4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>542</v>
+      </c>
+      <c r="D5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>543</v>
+      </c>
+      <c r="D6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>550</v>
+      </c>
+      <c r="D7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>551</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>545</v>
+      </c>
+      <c r="D14" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>546</v>
+      </c>
+      <c r="D17" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>547</v>
+      </c>
+      <c r="D20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>545</v>
+      </c>
+      <c r="D21" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>526</v>
+      </c>
+      <c r="D22" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>548</v>
+      </c>
+      <c r="D23" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>542</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>549</v>
+      </c>
+      <c r="D25" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>540</v>
+      </c>
+      <c r="D26" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CC965D-EE8C-4C55-BFCD-FB22F80E18F6}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B4" s="8">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" s="8">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="8">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="8">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="B12" s="8">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>